<commit_message>
Minor Update to Script
</commit_message>
<xml_diff>
--- a/Project Management/Budget.xlsx
+++ b/Project Management/Budget.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MCurtis\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MCurtis\Documents\Dungeon-AR\Project Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFECCBB0-4EA6-4F97-AAF5-22607F312B1F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CAAE196-15B3-4112-B2FE-9C97CABE84B1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-150" windowWidth="29040" windowHeight="16440" xr2:uid="{D131701E-58A9-4677-B268-649B95DC0020}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D131701E-58A9-4677-B268-649B95DC0020}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -574,7 +574,7 @@
   <dimension ref="B1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -801,6 +801,18 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C3:C16">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finalised budget document with prototype card printing cost as well as estimate on travel costs to convention. Total of £4800 suggested to round to £5000
</commit_message>
<xml_diff>
--- a/Project Management/Budget.xlsx
+++ b/Project Management/Budget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MCurtis\Documents\Dungeon-AR\Project Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CAAE196-15B3-4112-B2FE-9C97CABE84B1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B569E245-A4AB-4F43-AC9B-6B5B41E68B02}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D131701E-58A9-4677-B268-649B95DC0020}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Item</t>
   </si>
@@ -78,9 +78,6 @@
     <t>To charge showcasing phones when away from the studio</t>
   </si>
   <si>
-    <t>Quote to be obtained</t>
-  </si>
-  <si>
     <t>Krita</t>
   </si>
   <si>
@@ -124,6 +121,15 @@
   </si>
   <si>
     <t>To create licensed 3D Model assets with great textures, refer to Blender Plugin Document for details</t>
+  </si>
+  <si>
+    <t>This is just for the intial prototype run of 18 decks of 30 cards for use in showcasing and testing</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Rounded</t>
   </si>
 </sst>
 </file>
@@ -246,7 +252,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -256,6 +262,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -571,10 +578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7064C915-EC4E-4176-A31C-48689753FA4C}">
-  <dimension ref="B1:F28"/>
+  <dimension ref="B1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,14 +606,14 @@
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="7">
         <f>40+59+10</f>
         <v>109</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
@@ -650,7 +657,7 @@
         <v>156</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
@@ -658,10 +665,10 @@
         <v>10</v>
       </c>
       <c r="C8" s="8">
-        <v>0</v>
+        <v>210</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
@@ -688,116 +695,127 @@
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" s="8">
         <v>0</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" s="8">
         <v>1688</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="8">
-        <v>390</v>
+        <v>500</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="8">
         <v>1468</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" s="8">
         <f>6*12</f>
         <v>72</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" s="8">
         <f>9*6</f>
         <v>54</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="3"/>
       <c r="C17" s="8"/>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
       <c r="C18" s="8"/>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
       <c r="C19" s="8"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
       <c r="C20" s="8"/>
       <c r="D20" s="3"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="3"/>
       <c r="C21" s="8"/>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="3"/>
       <c r="C22" s="8"/>
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="3"/>
       <c r="C23" s="8"/>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
       <c r="C24" s="8"/>
       <c r="D24" s="3"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F28" s="6">
         <f>SUM(C3:C24)</f>
-        <v>4552</v>
+        <v>4872</v>
+      </c>
+      <c r="G28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F29" s="9">
+        <v>5000</v>
+      </c>
+      <c r="G29" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Slight edit to the budget to allow for cost changes, and uploaded test AR recognisable images
</commit_message>
<xml_diff>
--- a/Project Management/Budget.xlsx
+++ b/Project Management/Budget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MCurtis\Documents\Dungeon-AR\Project Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B569E245-A4AB-4F43-AC9B-6B5B41E68B02}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B780BCA9-E225-453D-B01F-EFFCC5D41259}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D131701E-58A9-4677-B268-649B95DC0020}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Item</t>
   </si>
@@ -129,7 +129,10 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Rounded</t>
+    <t>2D Artist</t>
+  </si>
+  <si>
+    <t>A small budget for commissioning 2D art for front and backs of cards</t>
   </si>
 </sst>
 </file>
@@ -252,7 +255,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -263,6 +266,7 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -581,7 +585,7 @@
   <dimension ref="B1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -762,9 +766,15 @@
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="3"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="3"/>
+      <c r="B17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="8">
+        <v>250</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
@@ -804,7 +814,7 @@
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F28" s="6">
         <f>SUM(C3:C24)</f>
-        <v>4872</v>
+        <v>5122</v>
       </c>
       <c r="G28" t="s">
         <v>31</v>
@@ -812,14 +822,26 @@
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F29" s="9">
-        <v>5000</v>
-      </c>
-      <c r="G29" t="s">
-        <v>32</v>
+        <v>7500</v>
+      </c>
+      <c r="G29" s="10">
+        <v>1.5</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C3:C16">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:C17">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>